<commit_message>
Add third (setup) button
</commit_message>
<xml_diff>
--- a/characters_code_generator.xlsx
+++ b/characters_code_generator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\Desktop\CO2-HopCannon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B62AE62-652D-4DA4-87FD-F130188F3490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F16353-66CD-474C-B4C1-D25964412E74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -161,7 +161,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
@@ -176,137 +175,7 @@
     <cellStyle name="Collegamento ipertestuale visitato" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1152,17 +1021,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A10:H13 F2:H9">
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:G26">
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:E9">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1180,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4525EBF9-8EBF-4E00-A9AA-3AE5C5CB384F}">
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="62" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="62" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
@@ -1260,16 +1129,16 @@
         <v>1</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
         <v>0</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -1322,19 +1191,19 @@
         <v>1</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1384,18 +1253,18 @@
         <v>1</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <v>0</v>
       </c>
       <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5" s="6">
-        <v>0</v>
-      </c>
-      <c r="W5" s="6">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
         <v>0</v>
       </c>
       <c r="X5" s="2"/>
@@ -1867,28 +1736,28 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <v>0</v>
@@ -1929,31 +1798,31 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15">
         <v>0</v>
@@ -1991,28 +1860,28 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -2223,7 +2092,7 @@
     </row>
     <row r="21" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
-        <f t="shared" ref="A21:L28" si="0">"B"&amp;A3&amp;B3&amp;C3&amp;D3&amp;E3</f>
+        <f t="shared" ref="A21:G28" si="0">"B"&amp;A3&amp;B3&amp;C3&amp;D3&amp;E3</f>
         <v>B00111</v>
       </c>
       <c r="G21" t="str">
@@ -2235,8 +2104,8 @@
         <v>B11111</v>
       </c>
       <c r="S21" t="str">
-        <f t="shared" ref="N21:S28" si="1">"B"&amp;S3&amp;T3&amp;U3&amp;V3&amp;W3</f>
-        <v>B00000</v>
+        <f t="shared" ref="S21:S28" si="1">"B"&amp;S3&amp;T3&amp;U3&amp;V3&amp;W3</f>
+        <v>B10110</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2249,12 +2118,12 @@
         <v>B11111</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" ref="M22:M29" si="2">"B"&amp;M4&amp;N4&amp;O4&amp;P4&amp;Q4</f>
+        <f t="shared" ref="M22:M28" si="2">"B"&amp;M4&amp;N4&amp;O4&amp;P4&amp;Q4</f>
         <v>B11111</v>
       </c>
       <c r="S22" t="str">
         <f t="shared" si="1"/>
-        <v>B00000</v>
+        <v>B11111</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2272,7 +2141,7 @@
       </c>
       <c r="S23" t="str">
         <f t="shared" si="1"/>
-        <v>B00000</v>
+        <v>B10110</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2394,7 +2263,7 @@
         <v>B00000</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" ref="S29:S37" si="6">"B"&amp;S12&amp;T12&amp;U12&amp;V12&amp;W12</f>
+        <f t="shared" ref="S30:S37" si="6">"B"&amp;S12&amp;T12&amp;U12&amp;V12&amp;W12</f>
         <v>B00000</v>
       </c>
     </row>
@@ -2427,11 +2296,11 @@
       </c>
       <c r="M32" t="str">
         <f t="shared" si="5"/>
-        <v>B00000</v>
+        <v>B10110</v>
       </c>
       <c r="S32" t="str">
         <f t="shared" si="6"/>
-        <v>B00000</v>
+        <v>B11100</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2445,11 +2314,11 @@
       </c>
       <c r="M33" t="str">
         <f t="shared" si="5"/>
-        <v>B00000</v>
+        <v>B11111</v>
       </c>
       <c r="S33" t="str">
         <f t="shared" si="6"/>
-        <v>B00000</v>
+        <v>B11110</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2463,11 +2332,11 @@
       </c>
       <c r="M34" t="str">
         <f t="shared" si="5"/>
-        <v>B00000</v>
+        <v>B10110</v>
       </c>
       <c r="S34" t="str">
         <f t="shared" si="6"/>
-        <v>B00000</v>
+        <v>B11100</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2538,8 +2407,8 @@
         <v>byte custom_char_c[] = {B11111, B11111, B11111, B00000, B00000, B00000, B00000, B00000};</v>
       </c>
       <c r="S39" t="str">
-        <f t="shared" ref="S39:AW39" si="8">"byte custom_char_"&amp;S20&amp;"[] = {"&amp;S21&amp;", "&amp;S22&amp;", "&amp;S23&amp;", "&amp;S24&amp;", "&amp;S25&amp;", "&amp;S26&amp;", "&amp;S27&amp;", "&amp;S28&amp;"};"</f>
-        <v>byte custom_char_d[] = {B00000, B00000, B00000, B00000, B00000, B00000, B00000, B00000};</v>
+        <f t="shared" ref="S39" si="8">"byte custom_char_"&amp;S20&amp;"[] = {"&amp;S21&amp;", "&amp;S22&amp;", "&amp;S23&amp;", "&amp;S24&amp;", "&amp;S25&amp;", "&amp;S26&amp;", "&amp;S27&amp;", "&amp;S28&amp;"};"</f>
+        <v>byte custom_char_d[] = {B10110, B11111, B10110, B00000, B00000, B00000, B00000, B00000};</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2548,16 +2417,16 @@
         <v>byte custom_char_e[] = {B00000, B00000, B10111, B11111, B10111, B00000, B00000, B00000};</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" ref="G40:AW40" si="9">"byte custom_char_"&amp;G29&amp;"[] = {"&amp;G30&amp;", "&amp;G31&amp;", "&amp;G32&amp;", "&amp;G33&amp;", "&amp;G34&amp;", "&amp;G35&amp;", "&amp;G36&amp;", "&amp;G37&amp;"};"</f>
+        <f t="shared" ref="G40:S40" si="9">"byte custom_char_"&amp;G29&amp;"[] = {"&amp;G30&amp;", "&amp;G31&amp;", "&amp;G32&amp;", "&amp;G33&amp;", "&amp;G34&amp;", "&amp;G35&amp;", "&amp;G36&amp;", "&amp;G37&amp;"};"</f>
         <v>byte custom_char_f[] = {B00000, B00000, B10000, B11000, B10000, B00000, B00000, B00000};</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" si="9"/>
-        <v>byte custom_char_g[] = {B00000, B00000, B00000, B00000, B00000, B00000, B00000, B00000};</v>
+        <v>byte custom_char_g[] = {B00000, B00000, B10110, B11111, B10110, B00000, B00000, B00000};</v>
       </c>
       <c r="S40" t="str">
         <f t="shared" si="9"/>
-        <v>byte custom_char_h[] = {B00000, B00000, B00000, B00000, B00000, B00000, B00000, B00000};</v>
+        <v>byte custom_char_h[] = {B00000, B00000, B11100, B11110, B11100, B00000, B00000, B00000};</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2588,11 +2457,11 @@
         <v xml:space="preserve">byte custom_char_a[] = {B00111, B01111, B01111, B00111, B01101, B11011, B11110, B11100};
 byte custom_char_b[] = {B11111, B11111, B11111, B10010, B11100, B00000, B00000, B00000};
 byte custom_char_c[] = {B11111, B11111, B11111, B00000, B00000, B00000, B00000, B00000};
-byte custom_char_d[] = {B00000, B00000, B00000, B00000, B00000, B00000, B00000, B00000};
+byte custom_char_d[] = {B10110, B11111, B10110, B00000, B00000, B00000, B00000, B00000};
 byte custom_char_e[] = {B00000, B00000, B10111, B11111, B10111, B00000, B00000, B00000};
 byte custom_char_f[] = {B00000, B00000, B10000, B11000, B10000, B00000, B00000, B00000};
-byte custom_char_g[] = {B00000, B00000, B00000, B00000, B00000, B00000, B00000, B00000};
-byte custom_char_h[] = {B00000, B00000, B00000, B00000, B00000, B00000, B00000, B00000};
+byte custom_char_g[] = {B00000, B00000, B10110, B11111, B10110, B00000, B00000, B00000};
+byte custom_char_h[] = {B00000, B00000, B11100, B11110, B11100, B00000, B00000, B00000};
 </v>
       </c>
     </row>
@@ -2601,131 +2470,136 @@
     <mergeCell ref="A1:W1"/>
   </mergeCells>
   <conditionalFormatting sqref="A11:I11 F3:F10 F12:F15 N21:AW21 S22:S28 Y22:Y28 AE22:AE28 AK22:AK28 AQ22:AQ28 AW22:AW28 M21:M36 N29:AW29 S30:S36 Y30:Y36 AE30:AE36 AK30:AK36 AQ30:AQ36 AW30:AW36 A30:L36 A37:AW37 A21:L21 A22:A29 G22:G28 A39:AW39">
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="39" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="38" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:AC10 AD8">
-    <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y12:AC19 AD13">
-    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE3:AI10">
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE12:AI19 AJ13">
-    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK3:AO10 AP10">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK12:AO19">
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ12:AU19">
-    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW12:BA19">
-    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ3:AU10">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW3:BA10">
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC3:BG10">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC12:BG19">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI12:BM19">
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI3:BM10">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:AW41">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:W10">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S6:W10">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12:W19">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:E10">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:K10">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:Q10 R5">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:E19">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:K19">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12:Q19">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M12:Q19">
+  <conditionalFormatting sqref="S3:W5">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>